<commit_message>
SUCE MA BITE GERBER
</commit_message>
<xml_diff>
--- a/LM_Task.xlsx
+++ b/LM_Task.xlsx
@@ -742,7 +742,7 @@
         <v>849</v>
       </c>
       <c r="M5" s="2">
-        <v>549</v>
+        <v>576</v>
       </c>
       <c r="N5" s="2" t="str">
         <v>1h</v>
@@ -757,7 +757,7 @@
         <v/>
       </c>
       <c r="R5" s="2">
-        <v>82350</v>
+        <v>86400</v>
       </c>
       <c r="S5" s="2">
         <v>150</v>
@@ -801,7 +801,7 @@
         <v>45</v>
       </c>
       <c r="M6" s="2">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="N6" s="2" t="str">
         <v>0</v>
@@ -816,7 +816,7 @@
         <v/>
       </c>
       <c r="R6" s="2">
-        <v>5400</v>
+        <v>9450</v>
       </c>
       <c r="S6" s="2">
         <v>150</v>
@@ -860,7 +860,7 @@
         <v>10</v>
       </c>
       <c r="M7" s="2">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N7" s="2" t="str">
         <v>1h</v>
@@ -875,7 +875,7 @@
         <v>Highest</v>
       </c>
       <c r="R7" s="2">
-        <v>2250</v>
+        <v>3600</v>
       </c>
       <c r="S7" s="2">
         <v>150</v>
@@ -919,7 +919,7 @@
         <v>10</v>
       </c>
       <c r="M8" s="2">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="N8" s="2" t="str">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>Highest</v>
       </c>
       <c r="R8" s="2">
-        <v>1800</v>
+        <v>3150</v>
       </c>
       <c r="S8" s="2">
         <v>0</v>
@@ -978,7 +978,7 @@
         <v>10</v>
       </c>
       <c r="M9" s="2">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="N9" s="2" t="str">
         <v>0</v>
@@ -993,7 +993,7 @@
         <v>Highest</v>
       </c>
       <c r="R9" s="2">
-        <v>1350</v>
+        <v>2700</v>
       </c>
       <c r="S9" s="2">
         <v>0</v>

</xml_diff>